<commit_message>
time to clean data
</commit_message>
<xml_diff>
--- a/main_extraction/main_fillings.xlsx
+++ b/main_extraction/main_fillings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jaison\Transfer\Jaison\MSPPM - DA\RAship\RAShip Tepper\Pandas Extraction\MAIN Extraction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pysol\Desktop\projects\sec_filings\main_extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D9864B-B3DF-4657-B259-13A7D39B9713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47D9374-9B4C-493E-A83C-265C5EEE27D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{578EB3AD-10A7-456F-B37A-B02DDF944409}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="11370" xr2:uid="{578EB3AD-10A7-456F-B37A-B02DDF944409}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="147">
   <si>
     <t>cik</t>
   </si>
@@ -462,6 +462,21 @@
   </si>
   <si>
     <t>Ending on Portfolio Investments</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1396440/000139644022000034/main-20220930.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1396440/000139644023000035/main-20221231.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1396440/000139644023000067/main-20230331.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1396440/000139644023000102/main-20230630.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1396440/000139644023000140/main-20230930.htm</t>
   </si>
 </sst>
 </file>
@@ -543,7 +558,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -553,6 +568,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -860,7 +877,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -868,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D55C8D7-4D48-4BE4-BDD7-431CB736F085}">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2260,6 +2277,106 @@
         <v>138</v>
       </c>
       <c r="J43" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="5">
+        <v>44869</v>
+      </c>
+      <c r="H44" t="s">
+        <v>142</v>
+      </c>
+      <c r="I44" t="s">
+        <v>138</v>
+      </c>
+      <c r="J44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="5">
+        <v>44981</v>
+      </c>
+      <c r="H45" t="s">
+        <v>143</v>
+      </c>
+      <c r="I45" t="s">
+        <v>138</v>
+      </c>
+      <c r="J45" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="5">
+        <v>45051</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="I46" t="s">
+        <v>138</v>
+      </c>
+      <c r="J46" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="5">
+        <v>45142</v>
+      </c>
+      <c r="H47" t="s">
+        <v>145</v>
+      </c>
+      <c r="I47" t="s">
+        <v>138</v>
+      </c>
+      <c r="J47" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="5">
+        <v>45233</v>
+      </c>
+      <c r="H48" t="s">
+        <v>146</v>
+      </c>
+      <c r="I48" t="s">
+        <v>138</v>
+      </c>
+      <c r="J48" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2356,6 +2473,7 @@
     <hyperlink ref="F43" r:id="rId89" xr:uid="{DF1671F6-66AD-4D8D-813C-FE38EF282BAA}"/>
     <hyperlink ref="G43" r:id="rId90" xr:uid="{6CE1FB17-8D96-4D8E-BCD3-2CBF93602A10}"/>
     <hyperlink ref="H43" r:id="rId91" xr:uid="{17B8E03A-0F89-45F4-8DDE-85EE2A2C06E2}"/>
+    <hyperlink ref="H46" r:id="rId92" xr:uid="{A770FC3F-47DE-4E29-9E45-8BB56B9FB25F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>